<commit_message>
Create workflow to trigger processing
</commit_message>
<xml_diff>
--- a/grupoetra/UC2.1 Network real-time monitoring.xlsx
+++ b/grupoetra/UC2.1 Network real-time monitoring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlacort\Documents\ETRA\Proyectos\BRIDGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BF89B2-4347-4DF6-BF48-8CAEC3528F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4493B0F-A4AD-4F8B-8920-28483A7AA6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
   <si>
     <t>1 Description of the use case</t>
   </si>
@@ -447,12 +447,6 @@
   </si>
   <si>
     <t>Energy</t>
-  </si>
-  <si>
-    <t>lkasjlfdks</t>
-  </si>
-  <si>
-    <t>werwer</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1294,18 +1288,14 @@
       <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>138</v>
-      </c>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>137</v>
-      </c>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>

</xml_diff>